<commit_message>
added end use calculation ´
</commit_message>
<xml_diff>
--- a/examples/End_Use_Technologies_DataBase.xlsx
+++ b/examples/End_Use_Technologies_DataBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiassteggemann/house-energy-mgmt-py/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FC8786-B0DC-C344-B24D-9297564D1E74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861A80AA-C05E-F047-A625-76E8E596149D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20140" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8660" yWindow="500" windowWidth="20140" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SpaceHeating" sheetId="1" r:id="rId1"/>
@@ -3261,7 +3261,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3320,7 +3320,7 @@
         <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>103</v>
+        <v>6</v>
       </c>
       <c r="C3" s="44">
         <v>6</v>

</xml_diff>